<commit_message>
Collections and Java8 intro
</commit_message>
<xml_diff>
--- a/Demo1-Intro/bin/resources/JavaTrainingRuffWork.xlsx
+++ b/Demo1-Intro/bin/resources/JavaTrainingRuffWork.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadbegum\Documents\JavaTraining\Java-Trainings\Demo1-Intro\src\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E07B34E-AF21-4AFE-85F2-581742AC6D18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1AAECFF-13A2-4829-94C0-C418EA59FD4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{49EA050B-88F9-4753-AA3A-E22E0DC8E5EA}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="101">
   <si>
     <t>Array/List</t>
   </si>
@@ -267,6 +267,75 @@
   </si>
   <si>
     <t>LInkedHashSet</t>
+  </si>
+  <si>
+    <t>SET</t>
+  </si>
+  <si>
+    <t>MAP</t>
+  </si>
+  <si>
+    <t>KEY</t>
+  </si>
+  <si>
+    <t>VALUE</t>
+  </si>
+  <si>
+    <t>MSD</t>
+  </si>
+  <si>
+    <t>LinkedList</t>
+  </si>
+  <si>
+    <t>Node</t>
+  </si>
+  <si>
+    <t>Hascode</t>
+  </si>
+  <si>
+    <t>Nxt node pointer</t>
+  </si>
+  <si>
+    <t>index:</t>
+  </si>
+  <si>
+    <t>hashcode</t>
+  </si>
+  <si>
+    <t>map.put--&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nxt node </t>
+  </si>
+  <si>
+    <t>map.get("MSD")</t>
+  </si>
+  <si>
+    <t>1. Match Hashcode</t>
+  </si>
+  <si>
+    <t>2. Match Content--&gt;equals check</t>
+  </si>
+  <si>
+    <t>......==…..</t>
+  </si>
+  <si>
+    <t>.quals check</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Sadiya</t>
+  </si>
+  <si>
+    <t>Raju</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hashcode and Equals </t>
   </si>
 </sst>
 </file>
@@ -305,7 +374,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -436,11 +505,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -457,6 +576,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -466,15 +594,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -789,20 +912,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{739F68A1-FCDA-4EFD-B427-17299D5A326D}">
-  <dimension ref="A5:N92"/>
+  <dimension ref="A5:P112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="F100" sqref="F100"/>
+    <sheetView tabSelected="1" topLeftCell="B94" workbookViewId="0">
+      <selection activeCell="I109" sqref="I109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.08984375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.453125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="4:14" x14ac:dyDescent="0.35">
@@ -1017,22 +1144,22 @@
       </c>
     </row>
     <row r="26" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G26" s="12"/>
-      <c r="H26" s="10" t="s">
+      <c r="G26" s="19"/>
+      <c r="H26" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I26" s="12"/>
-      <c r="J26" s="10" t="s">
+      <c r="I26" s="19"/>
+      <c r="J26" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="K26" s="12"/>
-      <c r="L26" s="10" t="s">
+      <c r="K26" s="19"/>
+      <c r="L26" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="M26" s="12"/>
+      <c r="M26" s="19"/>
     </row>
     <row r="27" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="F27" s="3"/>
@@ -1059,11 +1186,11 @@
       </c>
     </row>
     <row r="29" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G29" s="11"/>
-      <c r="H29" s="12"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="19"/>
     </row>
     <row r="30" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="H30" s="6" t="s">
@@ -1097,21 +1224,21 @@
       </c>
     </row>
     <row r="32" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F32" s="10" t="s">
+      <c r="F32" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G32" s="11"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="10" t="s">
+      <c r="G32" s="18"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="J32" s="11"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="10" t="s">
+      <c r="J32" s="18"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="M32" s="11"/>
-      <c r="N32" s="12"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="19"/>
     </row>
     <row r="35" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E35" t="s">
@@ -1274,10 +1401,10 @@
       <c r="G77" t="s">
         <v>54</v>
       </c>
-      <c r="H77" s="13" t="s">
+      <c r="H77" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="I77" s="13" t="s">
+      <c r="I77" s="10" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1311,7 +1438,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="81" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="81" spans="3:12" x14ac:dyDescent="0.35">
       <c r="H81" t="s">
         <v>53</v>
       </c>
@@ -1319,7 +1446,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="82" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="82" spans="3:12" x14ac:dyDescent="0.35">
       <c r="H82" t="s">
         <v>54</v>
       </c>
@@ -1327,7 +1454,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="83" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="83" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C83" t="s">
         <v>61</v>
       </c>
@@ -1350,7 +1477,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="84" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="84" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C84" t="s">
         <v>62</v>
       </c>
@@ -1361,21 +1488,21 @@
         <v>68</v>
       </c>
     </row>
-    <row r="85" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="H85" s="13" t="s">
+    <row r="85" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="H85" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="I85" s="14" t="s">
+      <c r="I85" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="J85" s="15" t="s">
+      <c r="J85" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="K85" s="18" t="s">
+      <c r="K85" s="16" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="86" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="86" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C86" t="s">
         <v>63</v>
       </c>
@@ -1385,15 +1512,15 @@
       <c r="E86" t="s">
         <v>66</v>
       </c>
-      <c r="I86" s="16" t="s">
+      <c r="I86" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="J86" s="17" t="s">
+      <c r="J86" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="K86" s="18"/>
-    </row>
-    <row r="87" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="K86" s="16"/>
+    </row>
+    <row r="87" spans="3:12" x14ac:dyDescent="0.35">
       <c r="I87" t="s">
         <v>73</v>
       </c>
@@ -1401,28 +1528,243 @@
         <v>74</v>
       </c>
     </row>
-    <row r="90" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="90" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D90" t="s">
         <v>75</v>
       </c>
-      <c r="F90" s="19" t="s">
+      <c r="F90" s="15" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="91" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="I90" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="91" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C91" t="s">
         <v>76</v>
       </c>
       <c r="E91" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="92" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="G91">
+        <v>15</v>
+      </c>
+      <c r="H91" s="9"/>
+      <c r="I91" t="s">
+        <v>72</v>
+      </c>
+      <c r="J91" t="s">
+        <v>72</v>
+      </c>
+      <c r="K91" t="s">
+        <v>72</v>
+      </c>
+      <c r="L91" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="92" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C92" t="s">
         <v>77</v>
       </c>
       <c r="E92" t="s">
         <v>38</v>
+      </c>
+      <c r="H92" s="9"/>
+    </row>
+    <row r="93" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="H93" s="9"/>
+    </row>
+    <row r="94" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="H94" s="9"/>
+    </row>
+    <row r="95" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="H95" s="9"/>
+    </row>
+    <row r="96" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D96" t="s">
+        <v>78</v>
+      </c>
+      <c r="H96" s="9"/>
+    </row>
+    <row r="97" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="D97" t="s">
+        <v>79</v>
+      </c>
+      <c r="H97" s="9"/>
+    </row>
+    <row r="98" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="C98" t="s">
+        <v>80</v>
+      </c>
+      <c r="D98" t="s">
+        <v>81</v>
+      </c>
+      <c r="H98" s="9"/>
+    </row>
+    <row r="99" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C99" t="s">
+        <v>82</v>
+      </c>
+      <c r="D99">
+        <v>100</v>
+      </c>
+      <c r="H99" s="9"/>
+    </row>
+    <row r="100" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G100">
+        <v>4</v>
+      </c>
+      <c r="H100" s="20"/>
+      <c r="I100" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="J100" s="22">
+        <v>1562557367</v>
+      </c>
+      <c r="K100" s="22">
+        <v>100</v>
+      </c>
+      <c r="L100" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="M100" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="N100" s="22">
+        <v>1262557367</v>
+      </c>
+      <c r="O100" s="22">
+        <v>99</v>
+      </c>
+      <c r="P100" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="101" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B101" t="s">
+        <v>87</v>
+      </c>
+      <c r="C101" t="s">
+        <v>88</v>
+      </c>
+      <c r="D101">
+        <v>1562557367</v>
+      </c>
+      <c r="E101">
+        <v>4</v>
+      </c>
+      <c r="G101">
+        <v>3</v>
+      </c>
+      <c r="H101" s="9"/>
+    </row>
+    <row r="102" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="G102">
+        <v>2</v>
+      </c>
+      <c r="H102" s="9"/>
+    </row>
+    <row r="103" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C103" t="s">
+        <v>89</v>
+      </c>
+      <c r="G103">
+        <v>1</v>
+      </c>
+      <c r="H103" s="9"/>
+    </row>
+    <row r="104" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G104">
+        <v>0</v>
+      </c>
+      <c r="H104" s="20"/>
+      <c r="I104" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="J104" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="K104" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="L104" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="M104" s="21"/>
+      <c r="N104" s="22"/>
+      <c r="O104" s="23"/>
+      <c r="P104" s="23"/>
+    </row>
+    <row r="105" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="C105" t="s">
+        <v>52</v>
+      </c>
+      <c r="D105">
+        <v>99</v>
+      </c>
+      <c r="K105" t="s">
+        <v>84</v>
+      </c>
+      <c r="N105" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="106" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="D106">
+        <v>1262557367</v>
+      </c>
+      <c r="E106">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="I107" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="108" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="C108" t="s">
+        <v>91</v>
+      </c>
+      <c r="I108" t="s">
+        <v>97</v>
+      </c>
+      <c r="J108" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="109" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="D109" t="s">
+        <v>92</v>
+      </c>
+      <c r="F109" t="s">
+        <v>94</v>
+      </c>
+      <c r="I109">
+        <v>101</v>
+      </c>
+      <c r="J109" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="110" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="D110" t="s">
+        <v>93</v>
+      </c>
+      <c r="F110" t="s">
+        <v>95</v>
+      </c>
+      <c r="I110">
+        <v>102</v>
+      </c>
+      <c r="J110" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="112" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="I112" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>